<commit_message>
modified alex report script
</commit_message>
<xml_diff>
--- a/WatanyaPingTester/bin/Debug/res/sokhnaReport.xlsx
+++ b/WatanyaPingTester/bin/Debug/res/sokhnaReport.xlsx
@@ -581,7 +581,7 @@
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -609,13 +609,13 @@
         <v>6</v>
       </c>
       <c r="C2">
-        <v>100</v>
+        <v>99.83</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -626,13 +626,13 @@
         <v>8</v>
       </c>
       <c r="C3">
-        <v>100</v>
+        <v>99.83</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -643,13 +643,13 @@
         <v>9</v>
       </c>
       <c r="C4">
-        <v>100</v>
+        <v>99.81</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -660,13 +660,13 @@
         <v>11</v>
       </c>
       <c r="C5">
-        <v>100</v>
+        <v>99.88</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>0.06</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -677,13 +677,13 @@
         <v>12</v>
       </c>
       <c r="C6">
-        <v>100</v>
+        <v>99.88</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>0.06</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -714,10 +714,10 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <v>33.33</v>
+        <v>0.4</v>
       </c>
       <c r="E8">
-        <v>66.6666666666667</v>
+        <v>99.6</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -728,13 +728,13 @@
         <v>15</v>
       </c>
       <c r="C9">
-        <v>100</v>
+        <v>99.86</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -748,10 +748,10 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <v>33.33</v>
+        <v>0.45</v>
       </c>
       <c r="E10">
-        <v>66.6666666666667</v>
+        <v>99.55</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -796,13 +796,13 @@
         <v>23</v>
       </c>
       <c r="C13">
-        <v>100</v>
+        <v>99.87</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>0.06</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -830,13 +830,13 @@
         <v>25</v>
       </c>
       <c r="C15">
-        <v>100</v>
+        <v>99.87</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>0.06</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -864,13 +864,13 @@
         <v>29</v>
       </c>
       <c r="C17">
-        <v>100</v>
+        <v>99.85</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -898,13 +898,13 @@
         <v>31</v>
       </c>
       <c r="C19">
-        <v>100</v>
+        <v>99.81</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -932,13 +932,13 @@
         <v>35</v>
       </c>
       <c r="C21">
-        <v>100</v>
+        <v>99.83</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -949,13 +949,13 @@
         <v>36</v>
       </c>
       <c r="C22">
-        <v>100</v>
+        <v>99.83</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1068,13 +1068,13 @@
         <v>47</v>
       </c>
       <c r="C29">
-        <v>100</v>
+        <v>89.37</v>
       </c>
       <c r="D29">
-        <v>0</v>
+        <v>10.55</v>
       </c>
       <c r="E29">
-        <v>0</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1085,13 +1085,13 @@
         <v>48</v>
       </c>
       <c r="C30">
-        <v>100</v>
+        <v>89.4</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>10.54</v>
       </c>
       <c r="E30">
-        <v>0</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1102,13 +1102,13 @@
         <v>50</v>
       </c>
       <c r="C31">
-        <v>100</v>
+        <v>89.37</v>
       </c>
       <c r="D31">
-        <v>0</v>
+        <v>10.55</v>
       </c>
       <c r="E31">
-        <v>0</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1136,13 +1136,13 @@
         <v>52</v>
       </c>
       <c r="C33">
-        <v>100</v>
+        <v>89.39</v>
       </c>
       <c r="D33">
-        <v>0</v>
+        <v>10.54</v>
       </c>
       <c r="E33">
-        <v>0</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1170,13 +1170,13 @@
         <v>56</v>
       </c>
       <c r="C35">
-        <v>100</v>
+        <v>89.41</v>
       </c>
       <c r="D35">
-        <v>0</v>
+        <v>10.53</v>
       </c>
       <c r="E35">
-        <v>0</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1187,13 +1187,13 @@
         <v>57</v>
       </c>
       <c r="C36">
-        <v>100</v>
+        <v>89.41</v>
       </c>
       <c r="D36">
-        <v>0</v>
+        <v>10.53</v>
       </c>
       <c r="E36">
-        <v>0</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1204,13 +1204,13 @@
         <v>59</v>
       </c>
       <c r="C37">
-        <v>100</v>
+        <v>89.42</v>
       </c>
       <c r="D37">
-        <v>0</v>
+        <v>10.52</v>
       </c>
       <c r="E37">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1221,13 +1221,13 @@
         <v>60</v>
       </c>
       <c r="C38">
-        <v>100</v>
+        <v>89.4</v>
       </c>
       <c r="D38">
-        <v>0</v>
+        <v>10.54</v>
       </c>
       <c r="E38">
-        <v>0</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1238,13 +1238,13 @@
         <v>62</v>
       </c>
       <c r="C39">
-        <v>100</v>
+        <v>89.36</v>
       </c>
       <c r="D39">
-        <v>0</v>
+        <v>10.54</v>
       </c>
       <c r="E39">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1255,13 +1255,13 @@
         <v>63</v>
       </c>
       <c r="C40">
-        <v>100</v>
+        <v>25.54</v>
       </c>
       <c r="D40">
-        <v>0</v>
+        <v>24.9</v>
       </c>
       <c r="E40">
-        <v>0</v>
+        <v>49.56</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1272,13 +1272,13 @@
         <v>64</v>
       </c>
       <c r="C41">
-        <v>100</v>
+        <v>89.14</v>
       </c>
       <c r="D41">
-        <v>0</v>
+        <v>10.6</v>
       </c>
       <c r="E41">
-        <v>0</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1289,13 +1289,13 @@
         <v>6</v>
       </c>
       <c r="C42">
-        <v>100</v>
+        <v>99.85</v>
       </c>
       <c r="D42">
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="E42">
-        <v>0</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1306,13 +1306,13 @@
         <v>66</v>
       </c>
       <c r="C43">
-        <v>0</v>
+        <v>21.02</v>
       </c>
       <c r="D43">
-        <v>100</v>
+        <v>78.959999999999994</v>
       </c>
       <c r="E43">
-        <v>0</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1323,13 +1323,13 @@
         <v>68</v>
       </c>
       <c r="C44">
-        <v>100</v>
+        <v>13.32</v>
       </c>
       <c r="D44">
-        <v>0</v>
+        <v>22.27</v>
       </c>
       <c r="E44">
-        <v>0</v>
+        <v>64.41</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1357,13 +1357,13 @@
         <v>70</v>
       </c>
       <c r="C46">
-        <v>0</v>
+        <v>12.93</v>
       </c>
       <c r="D46">
-        <v>33.33</v>
+        <v>22.4</v>
       </c>
       <c r="E46">
-        <v>66.6666666666667</v>
+        <v>64.680000000000007</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1374,13 +1374,13 @@
         <v>72</v>
       </c>
       <c r="C47">
-        <v>100</v>
+        <v>9.59</v>
       </c>
       <c r="D47">
-        <v>0</v>
+        <v>22.2</v>
       </c>
       <c r="E47">
-        <v>0</v>
+        <v>68.22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>